<commit_message>
Moved the management functions to the appropriate classes out of the GUI, added JOptionPane to the main JFrame
</commit_message>
<xml_diff>
--- a/ExcelFiles/TCconfig.xlsx
+++ b/ExcelFiles/TCconfig.xlsx
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,9 +715,6 @@
       <c r="A39" t="s">
         <v>40</v>
       </c>
-      <c r="B39" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -735,6 +732,9 @@
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>19</v>
+      </c>
+      <c r="B42" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>